<commit_message>
Amit made me do it
This is why he doesn't have a ring
</commit_message>
<xml_diff>
--- a/Winter_Appendix_data_fixed.xlsx
+++ b/Winter_Appendix_data_fixed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohan\Documents\GitHub\MCG4322B_Brace_Yourself\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE10D99-E0FE-4DF1-9875-1A2F9C05A938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B5FB7D-1CE8-44F4-9212-2088B4F4CD25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="817" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="817" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A1.Raw_Coordinate" sheetId="15" r:id="rId1"/>
@@ -1998,7 +1998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -20730,8 +20730,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AP110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="Q31" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="Z33" sqref="Z33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -37231,8 +37234,8 @@
   <dimension ref="A1:X111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P42" sqref="P42"/>
+      <pane ySplit="5" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -44596,11 +44599,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="S2:X2"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="C2:C4"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="A1:P1"/>
@@ -44610,6 +44608,11 @@
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="K2:P2"/>
     <mergeCell ref="D2:I2"/>
+    <mergeCell ref="S2:X2"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="C2:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>